<commit_message>
Necessary .xsls files to using prototype of .csv final file generator
</commit_message>
<xml_diff>
--- a/not_test_1.xlsx
+++ b/not_test_1.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\PycharmProjects\CSV_Creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4BACB4-D202-4D8C-93C5-823D42340420}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26480DDE-B85F-4A22-8F71-BE1525862B15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21855" yWindow="5895" windowWidth="15375" windowHeight="7875" xr2:uid="{5A818129-C0ED-4067-B196-02EC27236BB1}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A818129-C0ED-4067-B196-02EC27236BB1}"/>
   </bookViews>
   <sheets>
     <sheet name="not_tested" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">not_tested!$A$1:$D$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>null</t>
   </si>
@@ -428,7 +431,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,6 +451,9 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -459,6 +465,9 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -470,6 +479,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
@@ -478,17 +493,26 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
+      <c r="C5">
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -497,6 +521,9 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -508,6 +535,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -519,6 +549,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D8" xr:uid="{F7A7DE18-6B71-4112-AE31-5948B10155FA}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>